<commit_message>
Added 09. Defensive Programming and Exceptions
The Exercise and Homework are not yet added
</commit_message>
<xml_diff>
--- a/High-Quality Code/Useful Resources/Course Schedule.xlsx
+++ b/High-Quality Code/Useful Resources/Course Schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735"/>
@@ -238,11 +238,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\ mmm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,38 +321,38 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
       <numFmt numFmtId="164" formatCode="dd\ mmm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd\ mmm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -645,26 +645,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -674,7 +673,7 @@
     <col min="11" max="11" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
@@ -706,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -740,7 +739,7 @@
       </c>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -774,7 +773,7 @@
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -810,7 +809,7 @@
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -845,7 +844,7 @@
       </c>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -881,7 +880,7 @@
       </c>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -913,7 +912,7 @@
       </c>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -945,7 +944,7 @@
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -981,7 +980,7 @@
       </c>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -1017,7 +1016,7 @@
       </c>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>6</v>
       </c>
@@ -1050,7 +1049,7 @@
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -1083,7 +1082,7 @@
       </c>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>7</v>
       </c>
@@ -1116,7 +1115,7 @@
       </c>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>8</v>
       </c>
@@ -1148,7 +1147,7 @@
       </c>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>9</v>
       </c>
@@ -1180,7 +1179,7 @@
       </c>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>9</v>
       </c>
@@ -1212,7 +1211,7 @@
       </c>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>10</v>
       </c>
@@ -1248,7 +1247,7 @@
       </c>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>11</v>
       </c>
@@ -1280,7 +1279,7 @@
       </c>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>11</v>
       </c>
@@ -1316,7 +1315,7 @@
       </c>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>12</v>
       </c>
@@ -1348,7 +1347,7 @@
       </c>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>13</v>
       </c>
@@ -1380,7 +1379,7 @@
       </c>
       <c r="K21"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>14</v>
       </c>
@@ -1412,7 +1411,7 @@
       </c>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1439,7 +1438,7 @@
       </c>
       <c r="K23"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
@@ -1466,7 +1465,7 @@
       </c>
       <c r="K24"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1492,7 +1491,7 @@
       </c>
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>15</v>
       </c>
@@ -1517,7 +1516,7 @@
       </c>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added Defensive Programming and Exceptions Homework
</commit_message>
<xml_diff>
--- a/High-Quality Code/Useful Resources/Course Schedule.xlsx
+++ b/High-Quality Code/Useful Resources/Course Schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735"/>
@@ -238,11 +238,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\ mmm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,38 +321,38 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
       <numFmt numFmtId="164" formatCode="dd\ mmm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd\ mmm"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -645,21 +645,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.42578125" bestFit="1" customWidth="1"/>
@@ -669,11 +669,11 @@
     <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
@@ -705,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -739,7 +739,7 @@
       </c>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -773,7 +773,7 @@
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -809,7 +809,7 @@
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -844,7 +844,7 @@
       </c>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -880,7 +880,7 @@
       </c>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -912,7 +912,7 @@
       </c>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -944,7 +944,7 @@
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -980,7 +980,7 @@
       </c>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="2">
         <v>5</v>
       </c>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="2">
         <v>6</v>
       </c>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="2">
         <v>7</v>
       </c>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="2">
         <v>8</v>
       </c>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="2">
         <v>9</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="2">
         <v>9</v>
       </c>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="K16"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="2">
         <v>10</v>
       </c>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="2">
         <v>11</v>
       </c>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="2">
         <v>11</v>
       </c>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="2">
         <v>12</v>
       </c>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="2">
         <v>13</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="K21"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="2">
         <v>14</v>
       </c>
@@ -1411,7 +1411,7 @@
       </c>
       <c r="K22"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="K23"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="K24"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="2">
         <v>15</v>
       </c>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="B27" t="s">
         <v>28</v>
       </c>

</xml_diff>